<commit_message>
Se modifica Agregar Telas
</commit_message>
<xml_diff>
--- a/Agregar Telas/Añadir Campos.xlsx
+++ b/Agregar Telas/Añadir Campos.xlsx
@@ -20,21 +20,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">NOMBRE</t>
   </si>
   <si>
-    <t xml:space="preserve">dsadas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dasdasd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdasdsads</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ddsadasd</t>
+    <t xml:space="preserve">ALGODÓN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NYLON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POLIESTER</t>
   </si>
 </sst>
 </file>
@@ -44,7 +44,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -78,9 +78,22 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -125,7 +138,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -135,7 +148,19 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -158,12 +183,12 @@
   <dimension ref="A1:Z9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="72.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="56.01"/>
@@ -189,46 +214,44 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-      <c r="Y2" s="2"/>
-      <c r="Z2" s="2"/>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>2</v>
-      </c>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="J9" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Se añade mejora para subir también imagenes
</commit_message>
<xml_diff>
--- a/Agregar Telas/Añadir Campos.xlsx
+++ b/Agregar Telas/Añadir Campos.xlsx
@@ -20,21 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t xml:space="preserve">NOMBRE</t>
   </si>
   <si>
-    <t xml:space="preserve">ALGODÓN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NYLON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEDA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">POLIESTER</t>
+    <t xml:space="preserve">TINTE</t>
   </si>
 </sst>
 </file>
@@ -44,7 +35,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -88,12 +79,6 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -138,7 +123,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -153,10 +138,6 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -183,10 +164,10 @@
   <dimension ref="A1:Z9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="72.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.73"/>
@@ -224,22 +205,16 @@
       <c r="Z2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>2</v>
-      </c>
+      <c r="A3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="A4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5"/>
+      <c r="A6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>